<commit_message>
feat: working push products demo
</commit_message>
<xml_diff>
--- a/src/files/product-feed.xlsx
+++ b/src/files/product-feed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25318"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8B59861-950F-40D6-B278-07D589AF3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{551AD112-CBB7-4DEB-AC35-94C008CCEE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
   <si>
     <t>productGroupId</t>
   </si>
@@ -98,9 +98,6 @@
     <t>upc</t>
   </si>
   <si>
-    <t>brandName</t>
-  </si>
-  <si>
     <t>productTags_enUS</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Ombori</t>
-  </si>
-  <si>
     <t>Shirt,Black</t>
   </si>
   <si>
@@ -197,7 +191,7 @@
     <t>201</t>
   </si>
   <si>
-    <t>1-001-002</t>
+    <t>1-001,1-001-002</t>
   </si>
   <si>
     <t>Sweatpants</t>
@@ -726,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,13 +748,12 @@
     <col min="21" max="21" width="15.85546875" customWidth="1"/>
     <col min="22" max="22" width="24.85546875" customWidth="1"/>
     <col min="23" max="23" width="20.85546875" customWidth="1"/>
-    <col min="24" max="24" width="25.85546875" customWidth="1"/>
-    <col min="25" max="25" width="17.85546875" customWidth="1"/>
-    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" customWidth="1"/>
+    <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,288 +832,273 @@
       <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
       </c>
       <c r="K2">
         <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
         <v>37</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
       </c>
       <c r="Q2">
         <v>5</v>
       </c>
       <c r="R2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s">
+      <c r="X2" t="s">
         <v>40</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
       </c>
       <c r="K3">
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
         <v>37</v>
-      </c>
-      <c r="P3" t="s">
-        <v>38</v>
       </c>
       <c r="Q3">
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:26">
       <c r="A4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
       </c>
       <c r="K4">
         <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q4">
         <v>5</v>
       </c>
       <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="S4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>50</v>
       </c>
-      <c r="Z4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AA4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q5">
         <v>10</v>
       </c>
       <c r="R5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" t="s">
+        <v>44</v>
+      </c>
+      <c r="X5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="S5" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>50</v>
       </c>
-      <c r="Z5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA5" t="s">
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>59</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>60</v>
       </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" t="s">
-        <v>62</v>
-      </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6">
         <v>25</v>
@@ -1129,205 +1107,196 @@
         <v>20</v>
       </c>
       <c r="M6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="P6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q6">
         <v>2</v>
       </c>
       <c r="R6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" t="s">
-        <v>40</v>
-      </c>
       <c r="X6" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="Y6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z6" t="s">
         <v>66</v>
       </c>
-      <c r="Z6" t="s">
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="B7" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:27">
-      <c r="A7" s="5" t="s">
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>72</v>
       </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>73</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>74</v>
       </c>
-      <c r="H7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" t="s">
-        <v>76</v>
-      </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K7">
         <v>60</v>
       </c>
       <c r="M7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q7">
         <v>10</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="X7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="X7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>81</v>
       </c>
-      <c r="Z7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AA7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27">
-      <c r="A8" s="5" t="s">
+      <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>72</v>
       </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>73</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>74</v>
       </c>
-      <c r="H8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" t="s">
-        <v>76</v>
-      </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K8">
         <v>60</v>
       </c>
       <c r="M8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q8">
         <v>10</v>
       </c>
       <c r="R8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="X8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
         <v>85</v>
       </c>
-      <c r="X8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>88</v>
       </c>
-      <c r="E9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>89</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H9" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9">
         <v>15</v>
@@ -1336,25 +1305,22 @@
         <v>12</v>
       </c>
       <c r="M9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="P9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y9" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="P9" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" t="s">
-        <v>39</v>
-      </c>
-      <c r="X9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>94</v>
-      </c>
-      <c r="Z9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>